<commit_message>
Complete research update (dataset extended to 2024)
</commit_message>
<xml_diff>
--- a/data/raw/gdp_dataset.xlsx
+++ b/data/raw/gdp_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxisu/Desktop/gdp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxisu/Desktop/GDP-Time-Series-Forecasting/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E34488-DCB5-FD48-8475-02C7A359403E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3727578-EE72-024F-B0A4-C0BDF124E1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="25600" windowHeight="16000" xr2:uid="{111691B4-1E53-3945-A21E-5D96BBB656B8}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{111691B4-1E53-3945-A21E-5D96BBB656B8}"/>
   </bookViews>
   <sheets>
     <sheet name="季" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="707">
   <si>
     <t>71年第1季</t>
   </si>
@@ -2070,9 +2070,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>電力(企業)總用電量(十億度)</t>
-  </si>
-  <si>
     <t>進口物價基本分類指數</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2089,12 +2086,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>機械及電機設備進口值(十億元)</t>
-  </si>
-  <si>
-    <t>消費者物價指數</t>
-  </si>
-  <si>
     <t>失業率</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2124,6 +2115,67 @@
   </si>
   <si>
     <t>投資率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113年第1季</t>
+  </si>
+  <si>
+    <t>113年第2季</t>
+  </si>
+  <si>
+    <t>113年第3季</t>
+  </si>
+  <si>
+    <t>113年第4季</t>
+  </si>
+  <si>
+    <t>113年1月</t>
+  </si>
+  <si>
+    <t>113年2月</t>
+  </si>
+  <si>
+    <t>113年3月</t>
+  </si>
+  <si>
+    <t>113年4月</t>
+  </si>
+  <si>
+    <t>113年5月</t>
+  </si>
+  <si>
+    <t>113年6月</t>
+  </si>
+  <si>
+    <t>113年7月</t>
+  </si>
+  <si>
+    <t>113年8月</t>
+  </si>
+  <si>
+    <t>113年9月</t>
+  </si>
+  <si>
+    <t>113年10月</t>
+  </si>
+  <si>
+    <t>113年11月</t>
+  </si>
+  <si>
+    <t>113年12月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電力(企業)總用電量(十億度)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>機械及電機設備進口值(十億元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消費者物價指數</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2135,7 +2187,7 @@
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2197,6 +2249,13 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2223,7 +2282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2259,6 +2318,12 @@
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2575,10 +2640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2064BE-20A8-AB4D-82AC-E1154E7EEDB9}">
-  <dimension ref="A1:S169"/>
+  <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="143" workbookViewId="0">
+      <selection activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2597,13 +2662,13 @@
         <v>169</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -5051,7 +5116,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:6">
       <c r="A145" s="2" t="s">
         <v>143</v>
       </c>
@@ -5067,8 +5132,9 @@
       <c r="E145" s="11">
         <v>19.54</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" s="13"/>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>144</v>
       </c>
@@ -5085,7 +5151,7 @@
         <v>21.37</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:6">
       <c r="A147" s="2" t="s">
         <v>145</v>
       </c>
@@ -5102,7 +5168,7 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:6">
       <c r="A148" s="2" t="s">
         <v>146</v>
       </c>
@@ -5119,7 +5185,7 @@
         <v>23.74</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:6">
       <c r="A149" s="2" t="s">
         <v>147</v>
       </c>
@@ -5136,7 +5202,7 @@
         <v>21.62</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:6">
       <c r="A150" s="2" t="s">
         <v>148</v>
       </c>
@@ -5153,7 +5219,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:6">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -5170,7 +5236,7 @@
         <v>23.38</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:6">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -5187,7 +5253,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:6">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -5204,7 +5270,7 @@
         <v>24.33</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
         <v>152</v>
       </c>
@@ -5221,7 +5287,7 @@
         <v>25.84</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:6">
       <c r="A155" s="2" t="s">
         <v>153</v>
       </c>
@@ -5238,7 +5304,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
         <v>154</v>
       </c>
@@ -5255,7 +5321,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:6">
       <c r="A157" s="2" t="s">
         <v>155</v>
       </c>
@@ -5272,7 +5338,7 @@
         <v>23.08</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:6">
       <c r="A158" s="2" t="s">
         <v>156</v>
       </c>
@@ -5289,7 +5355,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:6">
       <c r="A159" s="2" t="s">
         <v>157</v>
       </c>
@@ -5306,7 +5372,7 @@
         <v>28.18</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
         <v>158</v>
       </c>
@@ -5474,6 +5540,74 @@
       </c>
       <c r="E169" s="11">
         <v>23.06</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="B170" s="10">
+        <v>6111775</v>
+      </c>
+      <c r="C170" s="9">
+        <v>31.45</v>
+      </c>
+      <c r="D170" s="9">
+        <v>1536850</v>
+      </c>
+      <c r="E170" s="11">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="B171" s="10">
+        <v>6233160</v>
+      </c>
+      <c r="C171" s="9">
+        <v>32.35</v>
+      </c>
+      <c r="D171" s="9">
+        <v>1748574</v>
+      </c>
+      <c r="E171" s="11">
+        <v>28.05</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="B172" s="10">
+        <v>6437479</v>
+      </c>
+      <c r="C172" s="9">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="D172" s="9">
+        <v>1666148</v>
+      </c>
+      <c r="E172" s="11">
+        <v>25.88</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B173" s="10">
+        <v>6810440</v>
+      </c>
+      <c r="C173" s="9">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="D173" s="9">
+        <v>1877753</v>
+      </c>
+      <c r="E173" s="11">
+        <v>27.57</v>
       </c>
     </row>
   </sheetData>
@@ -5484,10 +5618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D95C325-E49D-DE4E-8FB9-C23A4F443011}">
-  <dimension ref="A1:O505"/>
+  <dimension ref="A1:P517"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="L504" zoomScale="206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P515" sqref="P515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5515,40 +5649,40 @@
         <v>675</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>684</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>685</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>686</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -29237,6 +29371,571 @@
       </c>
       <c r="O505" s="7">
         <v>90.8</v>
+      </c>
+    </row>
+    <row r="506" spans="1:15">
+      <c r="A506" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B506" s="7">
+        <v>91.63</v>
+      </c>
+      <c r="C506" s="8">
+        <v>92.86</v>
+      </c>
+      <c r="D506" s="8">
+        <v>13.14</v>
+      </c>
+      <c r="E506" s="7">
+        <v>110.31</v>
+      </c>
+      <c r="F506" s="7">
+        <v>109.34</v>
+      </c>
+      <c r="G506" s="7">
+        <v>1154028</v>
+      </c>
+      <c r="H506" s="7">
+        <v>1076273</v>
+      </c>
+      <c r="I506" s="8">
+        <v>462.99</v>
+      </c>
+      <c r="J506" s="7">
+        <v>106.59</v>
+      </c>
+      <c r="K506" s="7">
+        <v>3.31</v>
+      </c>
+      <c r="L506" s="7">
+        <v>11587</v>
+      </c>
+      <c r="M506" s="7">
+        <v>23262</v>
+      </c>
+      <c r="N506" s="7">
+        <v>95.72</v>
+      </c>
+      <c r="O506" s="7">
+        <v>92.19</v>
+      </c>
+    </row>
+    <row r="507" spans="1:15">
+      <c r="A507" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B507" s="7">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C507" s="8">
+        <v>74.55</v>
+      </c>
+      <c r="D507" s="8">
+        <v>11.61</v>
+      </c>
+      <c r="E507" s="7">
+        <v>110.25</v>
+      </c>
+      <c r="F507" s="7">
+        <v>110.32</v>
+      </c>
+      <c r="G507" s="7">
+        <v>985596</v>
+      </c>
+      <c r="H507" s="7">
+        <v>737531</v>
+      </c>
+      <c r="I507" s="8">
+        <v>313</v>
+      </c>
+      <c r="J507" s="7">
+        <v>107.26</v>
+      </c>
+      <c r="K507" s="7">
+        <v>3.39</v>
+      </c>
+      <c r="L507" s="7">
+        <v>11572</v>
+      </c>
+      <c r="M507" s="7">
+        <v>23261</v>
+      </c>
+      <c r="N507" s="7">
+        <v>96.4</v>
+      </c>
+      <c r="O507" s="7">
+        <v>92.96</v>
+      </c>
+    </row>
+    <row r="508" spans="1:15">
+      <c r="A508" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B508" s="7">
+        <v>93.34</v>
+      </c>
+      <c r="C508" s="8">
+        <v>92.12</v>
+      </c>
+      <c r="D508" s="8">
+        <v>13.38</v>
+      </c>
+      <c r="E508" s="7">
+        <v>111.43</v>
+      </c>
+      <c r="F508" s="7">
+        <v>111.23</v>
+      </c>
+      <c r="G508" s="7">
+        <v>1319520</v>
+      </c>
+      <c r="H508" s="7">
+        <v>1044959</v>
+      </c>
+      <c r="I508" s="8">
+        <v>459.1</v>
+      </c>
+      <c r="J508" s="7">
+        <v>106.56</v>
+      </c>
+      <c r="K508" s="7">
+        <v>3.38</v>
+      </c>
+      <c r="L508" s="7">
+        <v>11581</v>
+      </c>
+      <c r="M508" s="7">
+        <v>23259</v>
+      </c>
+      <c r="N508" s="7">
+        <v>97.14</v>
+      </c>
+      <c r="O508" s="7">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="509" spans="1:15">
+      <c r="A509" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B509" s="7">
+        <v>87.88</v>
+      </c>
+      <c r="C509" s="8">
+        <v>89.88</v>
+      </c>
+      <c r="D509" s="8">
+        <v>13.55</v>
+      </c>
+      <c r="E509" s="7">
+        <v>113.88</v>
+      </c>
+      <c r="F509" s="7">
+        <v>113.46</v>
+      </c>
+      <c r="G509" s="7">
+        <v>1202135</v>
+      </c>
+      <c r="H509" s="7">
+        <v>1000965</v>
+      </c>
+      <c r="I509" s="8">
+        <v>481.42</v>
+      </c>
+      <c r="J509" s="7">
+        <v>107.15</v>
+      </c>
+      <c r="K509" s="7">
+        <v>3.36</v>
+      </c>
+      <c r="L509" s="7">
+        <v>11579</v>
+      </c>
+      <c r="M509" s="7">
+        <v>23258</v>
+      </c>
+      <c r="N509" s="7">
+        <v>97.93</v>
+      </c>
+      <c r="O509" s="7">
+        <v>94.92</v>
+      </c>
+    </row>
+    <row r="510" spans="1:15">
+      <c r="A510" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B510" s="7">
+        <v>98.02</v>
+      </c>
+      <c r="C510" s="8">
+        <v>95.16</v>
+      </c>
+      <c r="D510" s="8">
+        <v>14.65</v>
+      </c>
+      <c r="E510" s="7">
+        <v>113.39</v>
+      </c>
+      <c r="F510" s="7">
+        <v>113.52</v>
+      </c>
+      <c r="G510" s="7">
+        <v>1210113</v>
+      </c>
+      <c r="H510" s="7">
+        <v>1014693</v>
+      </c>
+      <c r="I510" s="8">
+        <v>471.11</v>
+      </c>
+      <c r="J510" s="7">
+        <v>107.38</v>
+      </c>
+      <c r="K510" s="7">
+        <v>3.34</v>
+      </c>
+      <c r="L510" s="7">
+        <v>11580</v>
+      </c>
+      <c r="M510" s="7">
+        <v>23256</v>
+      </c>
+      <c r="N510" s="7">
+        <v>98.7</v>
+      </c>
+      <c r="O510" s="7">
+        <v>95.93</v>
+      </c>
+    </row>
+    <row r="511" spans="1:15">
+      <c r="A511" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B511" s="7">
+        <v>93.96</v>
+      </c>
+      <c r="C511" s="8">
+        <v>89.94</v>
+      </c>
+      <c r="D511" s="8">
+        <v>14.31</v>
+      </c>
+      <c r="E511" s="7">
+        <v>113.79</v>
+      </c>
+      <c r="F511" s="7">
+        <v>113.21</v>
+      </c>
+      <c r="G511" s="7">
+        <v>1288938</v>
+      </c>
+      <c r="H511" s="7">
+        <v>1137231</v>
+      </c>
+      <c r="I511" s="8">
+        <v>530.85</v>
+      </c>
+      <c r="J511" s="7">
+        <v>107.71</v>
+      </c>
+      <c r="K511" s="7">
+        <v>3.39</v>
+      </c>
+      <c r="L511" s="7">
+        <v>11588</v>
+      </c>
+      <c r="M511" s="7">
+        <v>23255</v>
+      </c>
+      <c r="N511" s="7">
+        <v>99.36</v>
+      </c>
+      <c r="O511" s="7">
+        <v>96.84</v>
+      </c>
+    </row>
+    <row r="512" spans="1:15">
+      <c r="A512" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B512" s="7">
+        <v>96.11</v>
+      </c>
+      <c r="C512" s="8">
+        <v>95.69</v>
+      </c>
+      <c r="D512" s="8">
+        <v>15.15</v>
+      </c>
+      <c r="E512" s="7">
+        <v>114.41</v>
+      </c>
+      <c r="F512" s="7">
+        <v>114.3</v>
+      </c>
+      <c r="G512" s="7">
+        <v>1297542</v>
+      </c>
+      <c r="H512" s="7">
+        <v>1139668</v>
+      </c>
+      <c r="I512" s="8">
+        <v>567.36</v>
+      </c>
+      <c r="J512" s="7">
+        <v>107.92</v>
+      </c>
+      <c r="K512" s="7">
+        <v>3.45</v>
+      </c>
+      <c r="L512" s="7">
+        <v>11611</v>
+      </c>
+      <c r="M512" s="7">
+        <v>23253</v>
+      </c>
+      <c r="N512" s="7">
+        <v>99.89</v>
+      </c>
+      <c r="O512" s="7">
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16">
+      <c r="A513" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B513" s="7">
+        <v>102.59</v>
+      </c>
+      <c r="C513" s="8">
+        <v>97.72</v>
+      </c>
+      <c r="D513" s="8">
+        <v>15.42</v>
+      </c>
+      <c r="E513" s="7">
+        <v>112.87</v>
+      </c>
+      <c r="F513" s="7">
+        <v>113.09</v>
+      </c>
+      <c r="G513" s="7">
+        <v>1421771</v>
+      </c>
+      <c r="H513" s="7">
+        <v>1047023</v>
+      </c>
+      <c r="I513" s="8">
+        <v>496.44</v>
+      </c>
+      <c r="J513" s="7">
+        <v>108.34</v>
+      </c>
+      <c r="K513" s="7">
+        <v>3.48</v>
+      </c>
+      <c r="L513" s="7">
+        <v>11613</v>
+      </c>
+      <c r="M513" s="7">
+        <v>23250</v>
+      </c>
+      <c r="N513" s="7">
+        <v>100.23</v>
+      </c>
+      <c r="O513" s="7">
+        <v>98.22</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16">
+      <c r="A514" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B514" s="7">
+        <v>99.91</v>
+      </c>
+      <c r="C514" s="8">
+        <v>93.58</v>
+      </c>
+      <c r="D514" s="8">
+        <v>14.75</v>
+      </c>
+      <c r="E514" s="7">
+        <v>111.43</v>
+      </c>
+      <c r="F514" s="7">
+        <v>111.82</v>
+      </c>
+      <c r="G514" s="7">
+        <v>1298207</v>
+      </c>
+      <c r="H514" s="7">
+        <v>1070169</v>
+      </c>
+      <c r="I514" s="8">
+        <v>540.33000000000004</v>
+      </c>
+      <c r="J514" s="7">
+        <v>108.46</v>
+      </c>
+      <c r="K514" s="7">
+        <v>3.43</v>
+      </c>
+      <c r="L514" s="7">
+        <v>11604</v>
+      </c>
+      <c r="M514" s="7">
+        <v>23248</v>
+      </c>
+      <c r="N514" s="7">
+        <v>100.55</v>
+      </c>
+      <c r="O514" s="7">
+        <v>98.74</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16">
+      <c r="A515" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B515" s="7">
+        <v>100.55</v>
+      </c>
+      <c r="C515" s="8">
+        <v>94.11</v>
+      </c>
+      <c r="D515" s="8">
+        <v>14.4</v>
+      </c>
+      <c r="E515" s="7">
+        <v>111.29</v>
+      </c>
+      <c r="F515" s="7">
+        <v>111.98</v>
+      </c>
+      <c r="G515" s="7">
+        <v>1320910</v>
+      </c>
+      <c r="H515" s="7">
+        <v>1095742</v>
+      </c>
+      <c r="I515" s="8">
+        <v>576.22</v>
+      </c>
+      <c r="J515" s="7">
+        <v>108.73</v>
+      </c>
+      <c r="K515" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="L515" s="7">
+        <v>11609</v>
+      </c>
+      <c r="M515" s="7">
+        <v>23246</v>
+      </c>
+      <c r="N515" s="7">
+        <v>100.96</v>
+      </c>
+      <c r="O515" s="7">
+        <v>99.32</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" ht="19">
+      <c r="A516" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B516" s="7">
+        <v>102.49</v>
+      </c>
+      <c r="C516" s="8">
+        <v>95.09</v>
+      </c>
+      <c r="D516" s="8">
+        <v>13.82</v>
+      </c>
+      <c r="E516" s="7">
+        <v>111.28</v>
+      </c>
+      <c r="F516" s="7">
+        <v>112.39</v>
+      </c>
+      <c r="G516" s="7">
+        <v>1321674</v>
+      </c>
+      <c r="H516" s="7">
+        <v>1066289</v>
+      </c>
+      <c r="I516" s="8">
+        <v>545.30999999999995</v>
+      </c>
+      <c r="J516" s="7">
+        <v>108.84</v>
+      </c>
+      <c r="K516" s="7">
+        <v>3.36</v>
+      </c>
+      <c r="L516" s="7">
+        <v>11606</v>
+      </c>
+      <c r="M516" s="7">
+        <v>23245</v>
+      </c>
+      <c r="N516" s="7">
+        <v>101.49</v>
+      </c>
+      <c r="O516" s="7">
+        <v>100.12</v>
+      </c>
+      <c r="P516" s="12"/>
+    </row>
+    <row r="517" spans="1:16">
+      <c r="A517" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B517" s="7">
+        <v>108.39</v>
+      </c>
+      <c r="C517" s="8">
+        <v>98.97</v>
+      </c>
+      <c r="D517" s="8">
+        <v>13.35</v>
+      </c>
+      <c r="E517" s="7">
+        <v>111.76</v>
+      </c>
+      <c r="F517" s="7">
+        <v>112.94</v>
+      </c>
+      <c r="G517" s="7">
+        <v>1415108</v>
+      </c>
+      <c r="H517" s="7">
+        <v>1218339</v>
+      </c>
+      <c r="I517" s="8">
+        <v>626.54</v>
+      </c>
+      <c r="J517" s="7">
+        <v>108.82</v>
+      </c>
+      <c r="K517" s="7">
+        <v>3.32</v>
+      </c>
+      <c r="L517" s="7">
+        <v>11612</v>
+      </c>
+      <c r="M517" s="7">
+        <v>23244</v>
+      </c>
+      <c r="N517" s="7">
+        <v>102.07</v>
+      </c>
+      <c r="O517" s="7">
+        <v>101.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>